<commit_message>
Add more simulation results
</commit_message>
<xml_diff>
--- a/data/LCA Collection.xlsx
+++ b/data/LCA Collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Supply Chain Process" sheetId="1" state="visible" r:id="rId2"/>
@@ -381,13 +381,13 @@
     <t xml:space="preserve">Variant 1: </t>
   </si>
   <si>
-    <t xml:space="preserve">currogated box with kraft paper, lorry delivery and rerouting</t>
+    <t xml:space="preserve">carton board with kraft paper, lorry delivery and rerouting</t>
   </si>
   <si>
     <t xml:space="preserve">Variant 2: </t>
   </si>
   <si>
-    <t xml:space="preserve">currogated box with kraft paper, bike delivery and rerouting</t>
+    <t xml:space="preserve">carton board with kraft paper, bike delivery and rerouting</t>
   </si>
   <si>
     <t xml:space="preserve">Variant 3:</t>
@@ -842,11 +842,11 @@
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.28"/>
@@ -1065,7 +1065,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="3" t="n">
-        <f aca="false"> 0.0000139 * 2</f>
+        <f aca="false">0.0000139 * 2</f>
         <v>2.78E-005</v>
       </c>
     </row>
@@ -1096,11 +1096,11 @@
   </sheetPr>
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.04"/>
@@ -1211,7 +1211,7 @@
         <v>72</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>9.33E-005</v>
+        <v>0.000933</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>